<commit_message>
Plot new MS graph
</commit_message>
<xml_diff>
--- a/MS/Integrate/NO2PhO2SOPh/NO2PhO2SOPh-v1-v4-n.xlsx
+++ b/MS/Integrate/NO2PhO2SOPh/NO2PhO2SOPh-v1-v4-n.xlsx
@@ -60,7 +60,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -81,6 +81,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,18 +160,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -165,12 +187,12 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFF10D0C"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000CC"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF009900"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -263,18 +285,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.0" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -368,17 +379,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16617725"/>
-        <c:axId val="51140981"/>
+        <c:axId val="29247600"/>
+        <c:axId val="22926393"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16617725"/>
+        <c:axId val="29247600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -391,21 +402,28 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" lang="ru-RU" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51140981"/>
+        <c:crossAx val="22926393"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51140981"/>
+        <c:axId val="22926393"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,7 +438,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -433,16 +451,23 @@
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" lang="ru-RU" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16617725"/>
+        <c:crossAx val="29247600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -464,17 +489,6 @@
           <a:noFill/>
         </a:ln>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
@@ -494,16 +508,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>246600</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>275760</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>348840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -511,8 +525,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="246600" y="1281240"/>
-        <a:ext cx="5760000" cy="3241800"/>
+        <a:off x="591840" y="2313720"/>
+        <a:ext cx="5759640" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -533,21 +547,22 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.88"/>
@@ -566,7 +581,7 @@
       <c r="D1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -578,7 +593,7 @@
       <c r="H1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="0" t="s">
@@ -590,7 +605,7 @@
       <c r="L1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S1" s="0" t="s">
@@ -604,7 +619,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -616,7 +631,7 @@
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -628,7 +643,7 @@
       <c r="H2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="0" t="s">
@@ -640,18 +655,18 @@
       <c r="L2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -663,7 +678,7 @@
       <c r="D3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>10915.1</v>
       </c>
       <c r="F3" s="0" t="n">
@@ -675,7 +690,7 @@
       <c r="H3" s="0" t="n">
         <v>819.9</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="2" t="n">
         <v>8537.4</v>
       </c>
       <c r="J3" s="0" t="n">
@@ -687,20 +702,20 @@
       <c r="L3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="2" t="n">
         <v>10557.5</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <f aca="false">A3</f>
         <v>30</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="O3" s="4" t="n">
         <f aca="false">(E3+I3+M3)/3</f>
         <v>10003.3333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>60</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -712,7 +727,7 @@
       <c r="D4" s="0" t="n">
         <v>1196.7</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>9800</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -724,7 +739,7 @@
       <c r="H4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="2" t="n">
         <v>5762.2</v>
       </c>
       <c r="J4" s="0" t="n">
@@ -736,20 +751,20 @@
       <c r="L4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="2" t="n">
         <v>5320.2</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <f aca="false">A4</f>
         <v>60</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="O4" s="4" t="n">
         <f aca="false">(E4+I4+M4)/3</f>
         <v>6960.8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>90</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -761,7 +776,7 @@
       <c r="D5" s="0" t="n">
         <v>939.5</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <v>7685.8</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -773,7 +788,7 @@
       <c r="H5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="2" t="n">
         <v>5890.3</v>
       </c>
       <c r="J5" s="0" t="n">
@@ -785,20 +800,20 @@
       <c r="L5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="2" t="n">
         <v>6143.5</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <f aca="false">A5</f>
         <v>90</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="O5" s="4" t="n">
         <f aca="false">(E5+I5+M5)/3</f>
         <v>6573.2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>120</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -810,7 +825,7 @@
       <c r="D6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="2" t="n">
         <v>6282.8</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -822,7 +837,7 @@
       <c r="H6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="2" t="n">
         <v>5180.8</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -834,20 +849,20 @@
       <c r="L6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="2" t="n">
         <v>5603.4</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <f aca="false">A6</f>
         <v>120</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="O6" s="4" t="n">
         <f aca="false">(E6+I6+M6)/3</f>
         <v>5689</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>150</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -859,7 +874,7 @@
       <c r="D7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>4711.2</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -871,7 +886,7 @@
       <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="2" t="n">
         <v>4684</v>
       </c>
       <c r="J7" s="0" t="n">
@@ -883,20 +898,20 @@
       <c r="L7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="2" t="n">
         <v>4695.6</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <f aca="false">A7</f>
         <v>150</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="O7" s="4" t="n">
         <f aca="false">(E7+I7+M7)/3</f>
         <v>4696.93333333333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>180</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -908,7 +923,7 @@
       <c r="D8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="2" t="n">
         <v>7593.5</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -920,7 +935,7 @@
       <c r="H8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="2" t="n">
         <v>5976</v>
       </c>
       <c r="J8" s="0" t="n">
@@ -932,20 +947,20 @@
       <c r="L8" s="0" t="n">
         <v>245.1</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="2" t="n">
         <v>5924.5</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <f aca="false">A8</f>
         <v>180</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="O8" s="4" t="n">
         <f aca="false">(E8+I8+M8)/3</f>
         <v>6498</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>240</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -957,7 +972,7 @@
       <c r="D9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="2" t="n">
         <v>6760.7</v>
       </c>
       <c r="F9" s="0" t="n">
@@ -969,7 +984,7 @@
       <c r="H9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="2" t="n">
         <v>6764.9</v>
       </c>
       <c r="J9" s="0" t="n">
@@ -981,20 +996,20 @@
       <c r="L9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="2" t="n">
         <v>6188</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <f aca="false">A9</f>
         <v>240</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="O9" s="4" t="n">
         <f aca="false">(E9+I9+M9)/3</f>
         <v>6571.2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>300</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -1006,7 +1021,7 @@
       <c r="D10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="2" t="n">
         <v>7649.3</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -1018,7 +1033,7 @@
       <c r="H10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="2" t="n">
         <v>5991</v>
       </c>
       <c r="J10" s="0" t="n">
@@ -1030,20 +1045,20 @@
       <c r="L10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="2" t="n">
         <v>6834.6</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <f aca="false">A10</f>
         <v>300</v>
       </c>
-      <c r="O10" s="2" t="n">
+      <c r="O10" s="4" t="n">
         <f aca="false">(E10+I10+M10)/3</f>
         <v>6824.96666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>450</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -1055,7 +1070,7 @@
       <c r="D11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="2" t="n">
         <v>5901.6</v>
       </c>
       <c r="F11" s="0" t="n">
@@ -1067,7 +1082,7 @@
       <c r="H11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="2" t="n">
         <v>5329.5</v>
       </c>
       <c r="J11" s="0" t="n">
@@ -1079,20 +1094,20 @@
       <c r="L11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="2" t="n">
         <v>5703.1</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="1" t="n">
         <f aca="false">A11</f>
         <v>450</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="O11" s="4" t="n">
         <f aca="false">(E11+I11+M11)/3</f>
         <v>5644.73333333333</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>600</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -1104,7 +1119,7 @@
       <c r="D12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="2" t="n">
         <v>6323.3</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -1116,7 +1131,7 @@
       <c r="H12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="2" t="n">
         <v>6095.2</v>
       </c>
       <c r="J12" s="0" t="n">
@@ -1128,20 +1143,20 @@
       <c r="L12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="2" t="n">
         <v>6245.9</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <f aca="false">A12</f>
         <v>600</v>
       </c>
-      <c r="O12" s="2" t="n">
+      <c r="O12" s="4" t="n">
         <f aca="false">(E12+I12+M12)/3</f>
         <v>6221.46666666667</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>900</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -1153,7 +1168,7 @@
       <c r="D13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="2" t="n">
         <v>6877.3</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -1165,7 +1180,7 @@
       <c r="H13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="2" t="n">
         <v>6567.4</v>
       </c>
       <c r="J13" s="0" t="n">
@@ -1177,14 +1192,14 @@
       <c r="L13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="2" t="n">
         <v>6453.1</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="1" t="n">
         <f aca="false">A13</f>
         <v>900</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="O13" s="4" t="n">
         <f aca="false">(E13+I13+M13)/3</f>
         <v>6632.6</v>
       </c>

</xml_diff>